<commit_message>
Refatora projeto para arquitetura MVC (Nível 4)
</commit_message>
<xml_diff>
--- a/Moedas.xlsx
+++ b/Moedas.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E03F080-64A1-414F-9C96-2A58460E343D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="10515" windowHeight="6990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Moedas</t>
+  </si>
   <si>
     <t>EUR</t>
   </si>
@@ -31,14 +30,14 @@
     <t>BTC</t>
   </si>
   <si>
-    <t>Moedas</t>
+    <t>CAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,21 +74,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -127,7 +118,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -197,7 +188,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -370,36 +361,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>